<commit_message>
Updated design with correction on USB port control, added photos,...
</commit_message>
<xml_diff>
--- a/DM1098_LUX-D-LITE_DepthAI_USB3C/Docs/Assembly Outputs/BOM/BOM-DM1098LUXD-LITE(Production).xlsx
+++ b/DM1098_LUX-D-LITE_DepthAI_USB3C/Docs/Assembly Outputs/BOM/BOM-DM1098LUXD-LITE(Production).xlsx
@@ -592,7 +592,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -601,25 +601,8 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,11 +613,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -662,34 +640,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -989,14 +950,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34:K34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1010,1261 +966,1242 @@
     <col min="9" max="11" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="1">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="1">
         <v>19</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="1">
         <v>9</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="1">
         <v>1</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="1">
         <v>4</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="1">
         <v>3</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I19" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J19" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="K19" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="1">
         <v>14</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I22" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="1">
         <v>2</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="1">
         <v>1</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="1">
         <v>2</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I25" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="1">
         <v>1</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="1">
         <v>2</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I27" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-    </row>
-    <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="1">
         <v>4</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I28" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="1">
         <v>4</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I29" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-    </row>
-    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="1">
         <v>1</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="I30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-    </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="1">
         <v>1</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I31" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="J31" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="K31" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="1">
         <v>1</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="I32" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="J32" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="K32" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="1">
         <v>1</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I33" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="J33" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="K33" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="1">
         <v>1</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="G34" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H34" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="J34" s="7" t="s">
+      <c r="J34" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="K34" s="7" t="s">
+      <c r="K34" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="1">
         <v>1</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="I35" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-    </row>
-    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="1">
         <v>1</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="I36" s="3" t="s">
+      <c r="I36" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-    </row>
-    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="1">
         <v>1</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="H37" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="I37" s="3" t="s">
+      <c r="I37" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-    </row>
-    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="1">
         <v>1</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="I38" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="37" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>